<commit_message>
baselining for new work
</commit_message>
<xml_diff>
--- a/data/behavior_mapping.xlsx
+++ b/data/behavior_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harry/Uxpera/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1D4C0667-E6E2-CD47-B569-2E0FCBDA31E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B769769D-F3C0-0647-BAC7-DA65D2F7DD96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7400" yWindow="2400" windowWidth="22660" windowHeight="15280" xr2:uid="{EB95F2BC-F7D7-734A-983D-9E2D01404CA4}"/>
+    <workbookView xWindow="7400" yWindow="2400" windowWidth="30160" windowHeight="17940" xr2:uid="{EB95F2BC-F7D7-734A-983D-9E2D01404CA4}"/>
   </bookViews>
   <sheets>
     <sheet name="behavior_mapping" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>